<commit_message>
properly creates xaml files now
</commit_message>
<xml_diff>
--- a/Xaml_Maker/test.xlsx
+++ b/Xaml_Maker/test.xlsx
@@ -491,7 +491,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>BileDuct_Common</t>
+          <t>Bowel_Bag</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -504,7 +504,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>RGB0 240 0</t>
+          <t>RGB165 42 42</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -518,7 +518,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>71892</t>
+          <t>99</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -538,12 +538,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>BODY</t>
+          <t>SpinalCanal</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>EXTERNAL</t>
+          <t>ORGAN</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -551,7 +551,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>RGB0 255 0</t>
+          <t>RGB138255173</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -565,7 +565,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>256135</t>
+          <t>7647</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -585,7 +585,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Bowel_Bag</t>
+          <t>BileDuct_Common</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -598,7 +598,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>RGB165 42 42</t>
+          <t>RGB  0240  0</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -612,7 +612,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>71892</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -632,7 +632,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Bowel_Large</t>
+          <t>Heart</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -645,7 +645,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>RGB0 240 0</t>
+          <t>RGB255  0  0</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -659,7 +659,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>7201</t>
+          <t>7088</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -679,12 +679,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Bowel_Small</t>
+          <t>CTV</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>ORGAN</t>
+          <t>CTV</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -692,7 +692,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>RGB164 164 0</t>
+          <t>RGB255  0  0</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -706,7 +706,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>7200</t>
+          <t>88</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -726,12 +726,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Chestwall</t>
+          <t>CTV_High</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ORGAN</t>
+          <t>CTV</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -739,7 +739,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>RGB0 255 255</t>
+          <t>RGB255  0  0</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -753,7 +753,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>50060</t>
+          <t>88</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -773,20 +773,20 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>CTV_Low</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
           <t>CTV</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>CTV</t>
-        </is>
-      </c>
       <c r="D8" t="n">
         <v>2</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>RGB255 0 0</t>
+          <t>RGB255255  0</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -820,7 +820,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>CTV_High</t>
+          <t>CTV_Mid</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -833,7 +833,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>RGB255 0 0</t>
+          <t>RGB  6 82255</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -867,12 +867,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>CTV_Low</t>
+          <t>BODY</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>CTV</t>
+          <t>EXTERNAL</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -880,7 +880,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>RGB255 255 0</t>
+          <t>RGB  0255  0</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -894,7 +894,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>256135</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
@@ -914,12 +914,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>CTV_Mid</t>
+          <t>Duodenum</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>CTV</t>
+          <t>ORGAN</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -927,7 +927,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>RGB6 82 255</t>
+          <t>RGB233 67 67</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -941,7 +941,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>7206</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -961,7 +961,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Duodenum</t>
+          <t>Esophagus</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -974,7 +974,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>RGB233 67 67</t>
+          <t>RGB255165  0</t>
         </is>
       </c>
       <c r="F12" t="n">
@@ -988,7 +988,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>7206</t>
+          <t>7131</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -1008,7 +1008,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Esophagus</t>
+          <t>Stomach</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1021,7 +1021,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>RGB255 165 0</t>
+          <t>RGB164  0  0</t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -1035,7 +1035,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>7131</t>
+          <t>7148</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
@@ -1055,12 +1055,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>GallBladder</t>
+          <t>GTV</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>ORGAN</t>
+          <t>GTV</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -1068,7 +1068,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>RGB138 255 173</t>
+          <t>RGB  0240  0</t>
         </is>
       </c>
       <c r="F14" t="n">
@@ -1082,7 +1082,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>7202</t>
+          <t>88</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
@@ -1102,20 +1102,20 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
+          <t>GTVn</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
           <t>GTV</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>GTV</t>
-        </is>
-      </c>
       <c r="D15" t="n">
         <v>2</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>RGB0 240 0</t>
+          <t>RGB  0240  0</t>
         </is>
       </c>
       <c r="F15" t="n">
@@ -1149,7 +1149,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>GTVn</t>
+          <t>GTVp</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1162,7 +1162,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>RGB0 240 0</t>
+          <t>RGB  0240  0</t>
         </is>
       </c>
       <c r="F16" t="n">
@@ -1196,12 +1196,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>GTVp</t>
+          <t>Liver</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>GTV</t>
+          <t>ORGAN</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -1209,7 +1209,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>RGB0 240 0</t>
+          <t>RGB255165  0</t>
         </is>
       </c>
       <c r="F17" t="n">
@@ -1223,7 +1223,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>7197</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
@@ -1243,7 +1243,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Heart</t>
+          <t>Bowel_Small</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1256,7 +1256,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>RGB255 0 0</t>
+          <t>RGB164164  0</t>
         </is>
       </c>
       <c r="F18" t="n">
@@ -1270,7 +1270,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>7088</t>
+          <t>7200</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
@@ -1290,12 +1290,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>ITV</t>
+          <t>Bowel_Large</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>CTV</t>
+          <t>ORGAN</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -1303,7 +1303,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>RGB255 165 0</t>
+          <t>RGB  0240  0</t>
         </is>
       </c>
       <c r="F19" t="n">
@@ -1317,7 +1317,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>7201</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
@@ -1337,12 +1337,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Kidneys</t>
+          <t>ITV</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>ORGAN</t>
+          <t>CTV</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -1350,7 +1350,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>RGB0 119 170</t>
+          <t>RGB255165  0</t>
         </is>
       </c>
       <c r="F20" t="n">
@@ -1364,7 +1364,7 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>7203</t>
+          <t>88</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
@@ -1384,7 +1384,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Kidney_L</t>
+          <t>SpinalCord</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1397,7 +1397,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>RGB255 255 0</t>
+          <t>RGB  0240  0</t>
         </is>
       </c>
       <c r="F21" t="n">
@@ -1411,7 +1411,7 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>7205</t>
+          <t>7647</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
@@ -1431,7 +1431,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Kidney_R</t>
+          <t>Chestwall</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1444,7 +1444,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>RGB138 255 173</t>
+          <t>RGB  0255255</t>
         </is>
       </c>
       <c r="F22" t="n">
@@ -1458,7 +1458,7 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>7204</t>
+          <t>50060</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
@@ -1478,12 +1478,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Liver</t>
+          <t>PTV</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>ORGAN</t>
+          <t>PTV</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -1491,7 +1491,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>RGB255 165 0</t>
+          <t>RGB255  0  0</t>
         </is>
       </c>
       <c r="F23" t="n">
@@ -1505,7 +1505,7 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>7197</t>
+          <t>88</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
@@ -1525,12 +1525,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Lungs</t>
+          <t>PTV_High</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>ORGAN</t>
+          <t>PTV</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -1538,7 +1538,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>RGB6 82 255</t>
+          <t>RGB255  0  0</t>
         </is>
       </c>
       <c r="F24" t="n">
@@ -1552,7 +1552,7 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>7195</t>
+          <t>88</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
@@ -1572,12 +1572,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Lung_L</t>
+          <t>PTV_Low</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>ORGAN</t>
+          <t>PTV</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -1585,7 +1585,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>RGB127 255 212</t>
+          <t>RGB255255  0</t>
         </is>
       </c>
       <c r="F25" t="n">
@@ -1599,7 +1599,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>7310</t>
+          <t>88</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
@@ -1619,20 +1619,20 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
+          <t>PTV_Mid</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
           <t>PTV</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>PTV</t>
-        </is>
-      </c>
       <c r="D26" t="n">
         <v>2</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>RGB255 0 0</t>
+          <t>RGB  6 82255</t>
         </is>
       </c>
       <c r="F26" t="n">
@@ -1666,12 +1666,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>PTV_High</t>
+          <t>Lungs</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>PTV</t>
+          <t>ORGAN</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -1679,7 +1679,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>RGB255 0 0</t>
+          <t>RGB  6 82255</t>
         </is>
       </c>
       <c r="F27" t="n">
@@ -1693,7 +1693,7 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>7195</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
@@ -1713,12 +1713,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>PTV_Low</t>
+          <t>Lung_L</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>PTV</t>
+          <t>ORGAN</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -1726,7 +1726,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>RGB255 255 0</t>
+          <t>RGB127255212</t>
         </is>
       </c>
       <c r="F28" t="n">
@@ -1740,7 +1740,7 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>7310</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
@@ -1760,12 +1760,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>PTV_Mid</t>
+          <t>Kidneys</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>PTV</t>
+          <t>ORGAN</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -1773,7 +1773,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>RGB6 82 255</t>
+          <t>RGB  0119170</t>
         </is>
       </c>
       <c r="F29" t="n">
@@ -1787,7 +1787,7 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>7203</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
@@ -1807,7 +1807,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>SpinalCanal</t>
+          <t>Kidney_R</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1820,7 +1820,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>RGB138 255 173</t>
+          <t>RGB138255173</t>
         </is>
       </c>
       <c r="F30" t="n">
@@ -1834,7 +1834,7 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>7647</t>
+          <t>7204</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
@@ -1854,7 +1854,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>SpinalCord</t>
+          <t>Kidney_L</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1867,7 +1867,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>RGB0 240 0</t>
+          <t>RGB255255  0</t>
         </is>
       </c>
       <c r="F31" t="n">
@@ -1881,7 +1881,7 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>7647</t>
+          <t>7205</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
@@ -1901,7 +1901,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Stomach</t>
+          <t>GallBladder</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1914,7 +1914,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>RGB164 0 0</t>
+          <t>RGB138255173</t>
         </is>
       </c>
       <c r="F32" t="n">
@@ -1928,7 +1928,7 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>7148</t>
+          <t>7202</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
@@ -1961,7 +1961,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>RGB0 127 255</t>
+          <t>RGB  0127255</t>
         </is>
       </c>
       <c r="F33" t="n">

</xml_diff>

<commit_message>
RGB to segment names
</commit_message>
<xml_diff>
--- a/Xaml_Maker/test.xlsx
+++ b/Xaml_Maker/test.xlsx
@@ -645,7 +645,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>RGB255  0  0</t>
+          <t>Segment - Red</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -692,7 +692,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>RGB255  0  0</t>
+          <t>Segment - Red</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -739,7 +739,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>RGB255  0  0</t>
+          <t>Segment - Red</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -880,7 +880,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>RGB  0255  0</t>
+          <t>Segment - Green</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -1491,7 +1491,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>RGB255  0  0</t>
+          <t>Segment - Red</t>
         </is>
       </c>
       <c r="F23" t="n">
@@ -1538,7 +1538,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>RGB255  0  0</t>
+          <t>Segment - Red</t>
         </is>
       </c>
       <c r="F24" t="n">

</xml_diff>

<commit_message>
update top part to correctly list the date and description
</commit_message>
<xml_diff>
--- a/Xaml_Maker/test.xlsx
+++ b/Xaml_Maker/test.xlsx
@@ -491,7 +491,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Bowel_Bag</t>
+          <t>BileDuct_Common</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -504,7 +504,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>RGB165 42 42</t>
+          <t>RGB  0240  0</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -518,7 +518,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>71892</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -538,12 +538,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>SpinalCanal</t>
+          <t>BODY</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>ORGAN</t>
+          <t>EXTERNAL</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -551,7 +551,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>RGB138255173</t>
+          <t>Segment - Green</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -565,7 +565,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>7647</t>
+          <t>256135</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -585,7 +585,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>BileDuct_Common</t>
+          <t>Bowel_Bag</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -598,7 +598,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>RGB  0240  0</t>
+          <t>RGB165 42 42</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -612,7 +612,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>71892</t>
+          <t>99</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -632,7 +632,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Heart</t>
+          <t>Bowel_Large</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -645,7 +645,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Segment - Red</t>
+          <t>RGB  0240  0</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -659,7 +659,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>7088</t>
+          <t>7201</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -679,12 +679,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>CTV</t>
+          <t>Bowel_Small</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>CTV</t>
+          <t>ORGAN</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -692,7 +692,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Segment - Red</t>
+          <t>RGB164164  0</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -706,7 +706,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>7200</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -726,12 +726,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>CTV_High</t>
+          <t>Chestwall</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>CTV</t>
+          <t>ORGAN</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -739,7 +739,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Segment - Red</t>
+          <t>RGB  0255255</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -753,7 +753,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>50060</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -773,7 +773,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>CTV_Low</t>
+          <t>CTV</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -786,7 +786,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>RGB255255  0</t>
+          <t>Segment - Red</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -820,7 +820,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>CTV_Mid</t>
+          <t>CTV_High</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -833,7 +833,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>RGB  6 82255</t>
+          <t>Segment - Red</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -867,12 +867,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>BODY</t>
+          <t>CTV_Low</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>EXTERNAL</t>
+          <t>CTV</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -880,7 +880,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Segment - Green</t>
+          <t>RGB255255  0</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -894,7 +894,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>256135</t>
+          <t>88</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
@@ -914,12 +914,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Duodenum</t>
+          <t>CTV_Mid</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>ORGAN</t>
+          <t>CTV</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -927,7 +927,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>RGB233 67 67</t>
+          <t>RGB  6 82255</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -941,7 +941,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>7206</t>
+          <t>88</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -961,7 +961,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Esophagus</t>
+          <t>Duodenum</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -974,7 +974,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>RGB255165  0</t>
+          <t>RGB233 67 67</t>
         </is>
       </c>
       <c r="F12" t="n">
@@ -988,7 +988,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>7131</t>
+          <t>7206</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -1008,7 +1008,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Stomach</t>
+          <t>Esophagus</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1021,7 +1021,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>RGB164  0  0</t>
+          <t>RGB255165  0</t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -1035,7 +1035,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>7148</t>
+          <t>7131</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
@@ -1055,12 +1055,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>GTV</t>
+          <t>GallBladder</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>GTV</t>
+          <t>ORGAN</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -1068,7 +1068,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>RGB  0240  0</t>
+          <t>RGB138255173</t>
         </is>
       </c>
       <c r="F14" t="n">
@@ -1082,7 +1082,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>7202</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
@@ -1102,7 +1102,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>GTVn</t>
+          <t>GTV</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1149,7 +1149,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>GTVp</t>
+          <t>GTVn</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1196,12 +1196,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Liver</t>
+          <t>GTVp</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>ORGAN</t>
+          <t>GTV</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -1209,7 +1209,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>RGB255165  0</t>
+          <t>RGB  0240  0</t>
         </is>
       </c>
       <c r="F17" t="n">
@@ -1223,7 +1223,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>7197</t>
+          <t>88</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
@@ -1243,7 +1243,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Bowel_Small</t>
+          <t>Heart</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1256,7 +1256,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>RGB164164  0</t>
+          <t>Segment - Red</t>
         </is>
       </c>
       <c r="F18" t="n">
@@ -1270,7 +1270,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>7200</t>
+          <t>7088</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
@@ -1290,12 +1290,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Bowel_Large</t>
+          <t>ITV</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>ORGAN</t>
+          <t>CTV</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -1303,7 +1303,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>RGB  0240  0</t>
+          <t>RGB255165  0</t>
         </is>
       </c>
       <c r="F19" t="n">
@@ -1317,7 +1317,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>7201</t>
+          <t>88</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
@@ -1337,12 +1337,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>ITV</t>
+          <t>Kidneys</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>CTV</t>
+          <t>ORGAN</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -1350,7 +1350,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>RGB255165  0</t>
+          <t>RGB  0119170</t>
         </is>
       </c>
       <c r="F20" t="n">
@@ -1364,7 +1364,7 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>7203</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
@@ -1384,7 +1384,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>SpinalCord</t>
+          <t>Kidney_L</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1397,7 +1397,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>RGB  0240  0</t>
+          <t>RGB255255  0</t>
         </is>
       </c>
       <c r="F21" t="n">
@@ -1411,7 +1411,7 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>7647</t>
+          <t>7205</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
@@ -1431,7 +1431,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Chestwall</t>
+          <t>Kidney_R</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1444,7 +1444,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>RGB  0255255</t>
+          <t>RGB138255173</t>
         </is>
       </c>
       <c r="F22" t="n">
@@ -1458,7 +1458,7 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>50060</t>
+          <t>7204</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
@@ -1478,12 +1478,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>PTV</t>
+          <t>Liver</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>PTV</t>
+          <t>ORGAN</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -1491,7 +1491,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Segment - Red</t>
+          <t>RGB255165  0</t>
         </is>
       </c>
       <c r="F23" t="n">
@@ -1505,7 +1505,7 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>7197</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
@@ -1525,12 +1525,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>PTV_High</t>
+          <t>Lungs</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>PTV</t>
+          <t>ORGAN</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -1538,7 +1538,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Segment - Red</t>
+          <t>RGB  6 82255</t>
         </is>
       </c>
       <c r="F24" t="n">
@@ -1552,7 +1552,7 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>7195</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
@@ -1572,12 +1572,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>PTV_Low</t>
+          <t>Lung_L</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>PTV</t>
+          <t>ORGAN</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -1585,7 +1585,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>RGB255255  0</t>
+          <t>RGB127255212</t>
         </is>
       </c>
       <c r="F25" t="n">
@@ -1599,7 +1599,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>7310</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
@@ -1619,7 +1619,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>PTV_Mid</t>
+          <t>PTV</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1632,7 +1632,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>RGB  6 82255</t>
+          <t>Segment - Red</t>
         </is>
       </c>
       <c r="F26" t="n">
@@ -1666,12 +1666,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Lungs</t>
+          <t>PTV_High</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>ORGAN</t>
+          <t>PTV</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -1679,7 +1679,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>RGB  6 82255</t>
+          <t>Segment - Red</t>
         </is>
       </c>
       <c r="F27" t="n">
@@ -1693,7 +1693,7 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>7195</t>
+          <t>88</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
@@ -1713,12 +1713,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Lung_L</t>
+          <t>PTV_Low</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>ORGAN</t>
+          <t>PTV</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -1726,7 +1726,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>RGB127255212</t>
+          <t>RGB255255  0</t>
         </is>
       </c>
       <c r="F28" t="n">
@@ -1740,7 +1740,7 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>7310</t>
+          <t>88</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
@@ -1760,12 +1760,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Kidneys</t>
+          <t>PTV_Mid</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>ORGAN</t>
+          <t>PTV</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -1773,7 +1773,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>RGB  0119170</t>
+          <t>RGB  6 82255</t>
         </is>
       </c>
       <c r="F29" t="n">
@@ -1787,7 +1787,7 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>7203</t>
+          <t>88</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
@@ -1807,7 +1807,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Kidney_R</t>
+          <t>SpinalCanal</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1834,7 +1834,7 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>7204</t>
+          <t>7647</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
@@ -1854,7 +1854,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Kidney_L</t>
+          <t>SpinalCord</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1867,7 +1867,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>RGB255255  0</t>
+          <t>RGB  0240  0</t>
         </is>
       </c>
       <c r="F31" t="n">
@@ -1881,7 +1881,7 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>7205</t>
+          <t>7647</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
@@ -1901,7 +1901,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>GallBladder</t>
+          <t>Stomach</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1914,7 +1914,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>RGB138255173</t>
+          <t>RGB164  0  0</t>
         </is>
       </c>
       <c r="F32" t="n">
@@ -1928,7 +1928,7 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>7202</t>
+          <t>7148</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">

</xml_diff>